<commit_message>
Get daily reddit data: Tue Feb  6 08:08:47 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_02_11.xlsx
+++ b/data/2024_02_11.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C455"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,2624 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1ak4px2</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Ombre + French tip!</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ak4px2</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1ak4a57</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Year of the 🐲♥️🐉</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ak4a57</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1ak3llx</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Help! Nothing I put on my nails works it's like they repel everything.</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ak3llx/help_nothing_i_put_on_my_nails_works_its_like/</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1ak35ju</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>A few sets i have done in the last few months.</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ak35ju</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1ak2ndr</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>My top looks of 2023...how are you nail techs so damn talented, for real! Appreciate you for making me look so good.</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ak2ndr</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1ak1zrg</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Do I need long natural nails to try builder gel?</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ak1zrg/do_i_need_long_natural_nails_to_try_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1ak18wr</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Valentines Day French Manicure (ish)</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lis3r82y6wgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1ak15ab</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Interested in a the jelly nail trend!</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ak15ab</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1ak0oxs</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Valentine’s Day nails! ❤️💖</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ak0oxs</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1ak0a15</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>love blue, love grey.. so ofc i love blue-grey✨✨</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ak0a15</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1ak07zw</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>V day nails</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1jlz0a45xvgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1ak04xr</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Greyscale 😍</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hdgpa91dwvgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1ajzljb</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Valentines Nails 💅🏽</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajzljb</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1ajz03x</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>should dip be lifting less than a week later?</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajz03x</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1ajyuuh</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Simple valentines set</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/apfsm16ykvgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1ajy9ml</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>I'm a total newbie with bad natural nails... help?</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ajy9ml/im_a_total_newbie_with_bad_natural_nails_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1ajyk6u</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Nails based off of a weevil 🐞</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajyk6u</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1ajyj7b</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Shiny fire 🦹🏽‍♀️</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h9y8yfq5ivgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1ajy2sr</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Valentine mani inspired by tessa.lyn.nails on Instagram</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajy2sr</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1ajy06b</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Should I peal these or leave them</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t9o24mgpdvgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1ajxo83</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Recent valentine nails I've done</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajxo83</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1ajx4ps</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Valentines Day nails :)</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hfg73z9e6vgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1ajwy2e</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Polly gel. I like to think it looks a bit like a caramel latte</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajwy2e</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1ajw9ea</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>my valentines set! first time doing a french nail</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajw9ea</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1ajw3k1</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Trying something new 😊</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajw3k1</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1ajs9mi</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Stick on nails?</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ajs9mi/stick_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1ajvjn7</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Feeling absolutely gorgeous today!</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wqr1yc0ptugc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1ajsrfn</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>I want to get french nails, i don’t want the damage but i want long lasting. BIAB, SNS, or Acrylic??</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ajsrfn/i_want_to_get_french_nails_i_dont_want_the_damage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1ajtajj</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>My gel-x journey! Last photo is my current set that I just finished (:</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajtajj</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1ajvauu</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Why did this top coat dull my sparkles when it dried? I love how fast it dries and how protective it feels but it ruins my polish by its dull effect.</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajvauu</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1ajv5ka</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Gold Diamond Glitter Nails</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajv5ka</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1ajuhld</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Blueberry milk nails 🫐🥛</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mqaokmrnlugc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1ajqo4i</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Different Shape?</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajqo4i</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1ajsver</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>First time with builder gel. Trying to grow my natural nails out.</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sci5wrbu9ugc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1ajkxyc</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Anxiety=</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajkxyc</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1ajhhp0</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Looking for Dashing Diva Fastbond Dupe</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ajhhp0/looking_for_dashing_diva_fastbond_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1ajnzhq</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>What do I do if I don’t like the color of my nails the day after?</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vczte76tatgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1ajh7zp</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Eyeshadow on diy gel nails is the coolest thing ever</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajh7zp</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1ajc0ql</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Retention, home vs salon</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ajc0ql/retention_home_vs_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1ajr9sq</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Have you guys seen almond tips on flat nail beds? Do they look good?</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ajr9sq/have_you_guys_seen_almond_tips_on_flat_nail_beds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1ajr3fw</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Need help identifying product!</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/233c6jo0xtgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1ajqloo</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Press ons</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ajqloo/press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1ajpqjo</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Nail tips for super tiny hands?</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ajpqjo/nail_tips_for_super_tiny_hands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1ajoqlg</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>🩷 Pink Skittle 🩷</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajoqlg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1ajokq1</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Latest Press Ons</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajokq1</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1ajo5d4</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>February set</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k5qpbgc0ctgc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1ajn3zy</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Barbie Valentines Nails by me</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajn3zy</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1ajn1h3</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>How can I stop?</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajn1h3</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1ajn0l8</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Valentines Nails💖</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hbf56aow3tgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1ajmjy1</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>💚⛓️🖤</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d6baf5dr0tgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1ajlk7p</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Newest set</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/66bkxaeytsgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1ajkuw5</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>new nails yippiee!!!!</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajkuw5</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1ajklfr</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>First time for everything, so far have been just taking care of them myself and letting them grow out a bit. It is a bit daunting of a visit, so looking for generic idea of what to ask for, and maybe what shape do you think would suit me best? Thanks :D</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gflrwph2nsgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1ajkjr4</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Help request please</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajkjr4</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1ajkede</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Looking for a narrow skin rasp/file</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ajkede/looking_for_a_narrow_skin_raspfile/</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1ajkaju</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Had these nails on for a few weeks and decided to fill them in and add some iridescent chrome</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajkaju</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1ajjs87</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Did my nails for lunar new year</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/esatpui2hsgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1ajjjnw</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Early Valentine's nails ❤️</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2soi5d0afsgc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1ajj74n</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>A husband on a mission - Valentine's including something for my 25 year anniversary</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajj74n</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1ajj114</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Birthday set 🥰</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tgetx6i1bsgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1ajisis</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>i don't know what to ask at a nail salon</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ajisis/i_dont_know_what_to_ask_at_a_nail_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1ajhuw6</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>New Set</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8gdd0gf22sgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1ajgngl</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Fake toenail question</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ajgngl/fake_toenail_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1ajg4xm</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Love day mani 💘 I think its my favorite ever</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajg4xm</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1ajg0go</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Nail remedy</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/95snf1fhmrgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1ajfkl9</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Kind of girly, but i like it.😋🩷</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajfkl9</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1ajc8ku</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>I need help picking V-day nails!</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajc8ku</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1ajcc35</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Europe - 1st time at home UV gel nails</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fdz5ajungqgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1ajbyun</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>My swords set 🗡️ My nail artist is crazy good!</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajbyun</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1ajby90</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>My best French made by me</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajby90</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1ajbu5j</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>I’m in love with this my work 💅🏻💖🌸💞💓</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajbu5j</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1ak4s9f</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Another Valentine's Mani? 💖</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ak4s9f</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1ak4qmc</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Baby blue ombre with French on top!</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ak4qmc</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1ak3bc3</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Trying out a new brand and I’m really satisfied!</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ak3bc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1ak2ez9</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Had to take the picture look at that shift 💧</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ak2ez9</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1ak2aqm</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>It feels like my nails are wearing Rihanna’s Swarovski crystal dress</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ak2aqm</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1ak0vey</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Boolba giving the illusion that it’s GITD 💫</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8i93txeb3wgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1ak0smc</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Gel polish too transparent?</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ak0smc</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1ak06em</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>I am so puzzled</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ak06em</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1ajzxs2</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Zoya 10 for 25 shipment came in!</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajzxs2</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1ajz14u</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>What is the best "least toxic" nail polish brand for new nail tech?</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ajz14u/what_is_the_best_least_toxic_nail_polish_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1ajyh26</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>ILNP Opal Sunset</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajyh26</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1ajy5l5</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>ILNP Fairy Dust 🧚🏻‍♂️✨💕</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajy5l5</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1ajy1as</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Snake Mountain ✨️</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajy1as</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1ajxrsb</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Experimenting with acrylic paint markers</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bmrjy66sbvgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1ajxkaj</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Is Beyond Polish a scam?</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ajxkaj/is_beyond_polish_a_scam/</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1ajwy6w</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>This chrome is so good!!</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajwy6w</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1ajuyre</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>A very green BKL skittle!</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajuyre</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1ajtfb6</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Swamp Gloss - But Elijah Wood</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajtfb6</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1ajw2ao</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Gelatinous cube nails</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajw2ao</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1ajv9nr</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Was in a crème mood</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gtm8ejqirugc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1ajuchm</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Threads Your Friends Wove Together❣️</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajuchm</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1aju6dk</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Matchy-matchy with my nails and pen on a rainy Monday morning!</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1kr23rhejugc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1ajtm9k</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>flight of the monarchs</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajtm9k</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1ajt5wh</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Twins, just not the identical kind</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qrghlyxxbugc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1ajswav</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Content creators!!</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ajswav/content_creators/</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1ajstua</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>What to do next?</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ajstua/what_to_do_next/</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1ajsa32</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Do you file all your nails down if one breaks?</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajsa32</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1ajrn5r</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Did my own nails for the very first time!</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajrn5r</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1ajq5h9</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Question about ‘Acrylates Copolymer’ in normal nail polish, after suffering BIAB / Gel Nail Polish allergy</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajq5h9</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1ajps9c</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Using a sheer as a topper to add pizazz to my creme polishes</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1vg4gbgnntgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1ajpq7q</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Boolba Topper</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajpq7q</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1ajpn6k</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>February Mani #3: Now Thats More Like It...</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t6zsurpnmtgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1ajpl9e</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>{PR} So sparkly 🤩</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5rfei25amtgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1ajp1iz</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Less than perfect application but still cute and interesting!</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/stx8tox9itgc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1ajooml</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>🩷 Pink Skittle 🩷</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajooml</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1ajogrz</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Quick Stamping</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajogrz</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1ajog80</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Went with a subdued mini French today.</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajog80</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1ajoaw9</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Peely nails</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ajoaw9/peely_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1ajo8fu</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>I suffer from eczema and unfortunately I have developed an allergy to acrylic and gel polishes. I'm trying normal nail polish for the first time in a while! :))</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c8tqysqkctgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1ajo3li</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Maybe/plum skittle</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/te5n7cmmbtgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1ajo16j</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer Thistle and Thorn</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajo16j</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1ajnwi3</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Already on my second Valentines mani🤭😩</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajnwi3</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1ajnnex</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Double skittle!</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajnnex</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1ajn2vv</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Purjoi, WHY!? Nail oil pen suggestions?</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ajn2vv/purjoi_why_nail_oil_pen_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1ajmm6o</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Am I crazy if does this skittle work?</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/55hc7cw61tgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1ajm3iw</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Best Top Coat for Flakies? (Disregard my fake tan fail fingers)</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5yfx6dumxsgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1ajlyh3</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Jan PPU - the Fox Gloves are Off!</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajlyh3</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1ajlomu</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Looking for some advice on shaping &amp; apex</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajlomu</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1ajlctf</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>shades of purple (blurple?)</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajlctf</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1ajl19y</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Hearts on stems 💖🌿</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajl19y</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1ajkqc4</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>First try at stamping</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajkqc4</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1ajjzxb</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>It was good while it lasted</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajjzxb</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1ajjyh9</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>ILNP Sandy Baby seems like my neutral?</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajjyh9</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1ajjyay</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Perfect Blue glow magenta</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajjyay</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1ajjrhk</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>rogue lacquer - fire &amp; ice</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajjrhk</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1ajjboj</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Valentine’s Season Mani</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k1ak7goldsgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1ajj0k9</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>♥️Playing Cards♥️</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajj0k9</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1ajj0jm</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Pastel yellow</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ajj0jm/pastel_yellow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1ajijvn</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Long bendy thin nails!</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ajijvn/long_bendy_thin_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1aji66y</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>My nails bleed constantly and it hurts plus they flake off at the end? What can I do to fix them?</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kc919nql4sgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1ajhb25</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Early Valentine's Nails</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/888q9lshxrgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1ajgmfg</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>New nails new mug</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajgmfg</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1ajge1b</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t xml:space="preserve">"Did you know that was going to happen?" --my boyfriend </t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3rv934qsprgc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1ajf00p</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>M&amp;N Indie Polish - Botany Class</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajf00p</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1ajea0g</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>I'm not much of a red person, but...</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajea0g</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1ajdx10</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ajdx10/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1ajck7p</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Junior Lacquerista in the making 💗💛💚💙💜</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/orxpbm4njqgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1ajcjrd</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>So happy with my valentines/birthday month/SIL’s engagement party nails!</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajcjrd</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1aiyok8</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Peeling nails 😭</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h0p0s8egwmgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1ak4mmf</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Not no simple French!</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ak4mmf</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1ak4bpq</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Mushu nail art 🐲♥️🐉</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ak4bpq</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1ak1z1b</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Lucky Cat Nails</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ak1z1b</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1ajyci1</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Weevil nails 💅🏼</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bl7hbsbfgvgc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1ajwerk</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>The clear version is still my favourite, but when my 2 nails broke I had to go with some of your suggestions to try the white :)</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajwerk</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1ajvv8x</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>I’m obsessed with how these turned out! Done by me @jolley.nails.</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajvv8x</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1ajtxzo</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Some sparkly swirls, just for fun✨</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hywzv3xnhugc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1ajtso5</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>my very first valentine nails. any feedback?</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/upo41x0igugc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1ajt5j4</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Lunar new years</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ri6rpjjvbugc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1ajs2z4</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>What vibe do these give?</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajs2z4</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1ajn77i</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>'Snakes in the bush' Gel Nail design + Glow</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajn77i</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1ajmj20</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Pika pika</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajmj20</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1ajbwy8</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Look at the crazy Gel X I just got! ⚔️🗡️</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zbdtja47bqgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1ajbv3c</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>I did it 🤩💖</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ajbv3c</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Feb  7 08:07:30 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_02_11.xlsx
+++ b/data/2024_02_11.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C455"/>
+  <dimension ref="A1:C612"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8168,6 +8168,2675 @@
         </is>
       </c>
     </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1akxc8n</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Nail set help</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akxc8n</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1akx1ey</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>4~5 year old Nail Strengthener(Polish), safe to use?</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1akx1ey/45_year_old_nail_strengthenerpolish_safe_to_use/</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1akvimq</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Gender reveal party nail?</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akvimq</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1akv6u9</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Valentines Nails</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1peq3zw7j3hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1akv08m</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>New set! I just love animal print, and white can never fail</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fral7vqdh3hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1akuy4g</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Some recent at home nail art by me! Roast me 😂</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lqyqptlxg3hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1aktetl</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Help!!</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aktetl</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1akt1kv</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Spring nails in honor of Punxsutawney Phil not seeing his shadow</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akt1kv</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1akurjr</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>My thumb or what?!</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akurjr</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1akq3lw</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>wanted to share this cutesy little set i did today 🤭</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ucm03r46a2hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1akpukw</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Timeless</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c95i22h282hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1aknynh</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Finished set!</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a9mnvm7ct1hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1akma6m</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Nail Art Ideas for OPI’s Humidi-Tea or Cozu-melted in the Sun</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1akma6m/nail_art_ideas_for_opis_humiditea_or_cozumelted/</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1aktw7p</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Circus heart art</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rimd3i0373hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1akstkg</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Valentines nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bj7kdhr9x2hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1aksck0</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>💜✨</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aksck0</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1aks31h</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Coraline Vibes 💙☔️</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aks31h</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1akrsqo</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Tap Gel</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4l8jmgefo2hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1akr10r</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Gel or acrylic?</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1akr10r/gel_or_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1akqqlw</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Broke two nails over the weekend, so I slapped on some falsies.</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mll3ml3if2hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1akq858</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Definitely this color is a very good option and it looks great on me with any type of outfit.</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3etdfjd3b2hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1akq0jf</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Went with something simple this time. Took me about 8 hours lol. Ive been doing polygel on my own nails for 5 years now. When will i get quicker with it?</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akq0jf</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1akpw4j</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Should I redo these...</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akpw4j</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1akps7m</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Pink berry jellies!</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/syl7pczi72hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1akpi6i</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>First time trying press ons! It’s been a week and they’re still on. Got them from Amazon🥰</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akpi6i</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1akohjo</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>I’m in love with these nails</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3p4jqwrbx1hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1akofef</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>My nails over the years</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akofef</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1akoa76</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Valentine’s Day freestyle from today</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ja8w79sv1hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1aknjwv</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>my valentines nails 🩷🤍</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3vbtn076q1hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1akndj3</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Thank you!</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akndj3</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1akn8qw</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>First time doing Gel-x on my own!</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akn8qw</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1akmfjn</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Been a mail biter forever and have been growing for a month</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akmfjn</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1akmo7g</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Set I did on my friend yesterday</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akmo7g</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1akmrte</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>How do I avoid getting glitter in my top coat???</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akmrte</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1akmotr</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>gel on my natural nails - red w/ a bit of gold for lunar new year 🧧❤️</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hd8bnwtxj1hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1akmk97</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>My first time doing nail art</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/79z6utkzi1hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1akmc7c</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Peel off base?</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1akmc7c/peel_off_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1akm7ik</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Nails</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ta6o32gg1hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1akm1sd</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Hott pink nails for Valentine’s Day</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f5rosrhaf1hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1aklwhh</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>I’m loving this color 🩸 gel polish with gel overlay on natural nails</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/71sp41p8e1hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1aklt5i</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>New chrome nails</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aklt5i</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1aklt1w</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>I tried the coquette nail trend</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ko3x6ebjd1hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1aklaay</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Disco nails 🪩</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aklaay</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1akkuu6</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>V-day nails 💘</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mz8j1fxw61hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1akktgj</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Hello. I am getting nail extension for the first time im years. I have questions</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1akktgj/hello_i_am_getting_nail_extension_for_the_first/</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1akkd4c</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>First polygel attempt. How thick should the underside be?</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akkd4c</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1akkb2q</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Chrome powder 🩵</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5qf9wmb131hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1akka78</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Stained glass nails 💗</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akka78</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1akk9b3</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Classic red ❤️</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/10sdrcoo21hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1akk7cu</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>No file build 🖤</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akk7cu</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1akjt77</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>They’re a little grown out but I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b76g3ujgz0hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1akiz4i</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Press Ons (Which Glue)</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1akiz4i/press_ons_which_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1akf8tx</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>First ombre set, inspired by one of V's customisation options in Cyberpunk 2077</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akf8tx</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1akheh3</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Valentine’s Day Nails🩷</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akheh3</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1akgsjb</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Valentine’s Day Nails ❤️</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akgsjb</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1akgm0y</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Custom press-ons by me😊</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lnkig92lc0hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1akfwlu</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>love this set by @n40536 from IG. Help a complete newbie out, how to do this on my own (what are the steps? what to use?)</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xv6vkjci70hc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1akf44z</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Nail shaping + other tips?</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akf44z</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1ake7b5</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Tips on damage</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dzdvo5rsuzgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1akevf0</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Vday nails 🥰💖</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ha8s67cvzzgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1akd0v8</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>New to Acrylics</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1akd0v8/new_to_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1akehzh</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>My happy pinkish nails</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1akehzh/my_happy_pinkish_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1akbyi8</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Why do my acrylics always look so wide and sized wrong??</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akbyi8</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1akdy8c</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>first attempt at nail art! i designed these thinking of valentines' sprinkled cupcakes 🧁🩷 ft. my VERY shaky hands 😭</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akdy8c</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1akde88</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Purple and black shornaislties</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xqgk44ouozgc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1akcaw0</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>My new gels for February</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cdlaa6mdgzgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1akbs3k</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>What type of manicure should I get?</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1akbs3k/what_type_of_manicure_should_i_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1akbm7t</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>I've been bombed by Valloween posts lately so... Goth+cheesy?</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akbm7t</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1akbg57</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Valentine’s nails🎀💞</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akbg57</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1akao6b</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Painted some smexy valentine's nails for myself 💗</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akao6b</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1ak97sf</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Ridges on thumb nail</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ak97sf</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1ak94kg</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Still new to DIY but having fun w/ it</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a5i9h413qygc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1ak7lhd</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Issue with nails what to do?</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ak7lhd</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1ak7g55</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>A manicure without a manicure)</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wqmsfv658ygc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1ak22r2</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Looking for gel nail paint of this shade</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ak22r2</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1ak5jna</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Drusilla inspired nails 💅</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qvhs7zt9kxgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1ak01mj</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Nail ideas for my bday!!</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ak01mj/nail_ideas_for_my_bday/</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1ak0t7m</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Valentines set</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qgzovjwp2wgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1ak586c</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Nails to match my cat! (Cat pics included)</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ak586c</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1ak761c</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>A kid at my work said I needed pink nails</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r27ww8b85ygc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1ak6i97</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Chinese Lunar New Year Sculpted Dragons</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ak6i97</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1ak69ov</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Call out for UK based POC nail DIY-ers for a nationwide art project!</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ak69ov/call_out_for_uk_based_poc_nail_diyers_for_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1ak6250</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Absolutely love 2 tones like these</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h9sdvqu5rxgc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1ak5kdg</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Builder Gel</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/we8h0rnjkxgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1akx7cb</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>What I wore in January</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akx7cb</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1akvkmx</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>In love with baby blue ombre!</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akvkmx</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1akqsqh</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Pink is my favorite color 🩷 Polishes Used: ILNP (Shade: Misbehaving) | Essie (Shade: Gel Couture Top Coat)</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akqsqh</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1aku02w</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Cotton Candy Yeti - Lumen Nails Myths &amp; Monsters Yeti Mystery Polish</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aku02w</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1aktki3</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Minimal Valentine’s Day look on short nails</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ks46xyf143hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1aktbm1</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Color ID?</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/904nh0ds13hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1akt3hf</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Polish is my stress relief 💅- here are some looks/swatches I've done lately!</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akt3hf</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1akt3fz</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>need nail polish suggestions</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1akt3fz/need_nail_polish_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1akscb2</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>mooncat and seche vite</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1akscb2/mooncat_and_seche_vite/</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1akrzm3</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>New hobby</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akrzm3</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1akrvwt</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Got the Essie gel couture top coat because of this group. Now what are some of your favorite easy to work with sheer/natural polishes and glitter toppers?!</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1akrvwt/got_the_essie_gel_couture_top_coat_because_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1akqp60</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>adapt, improvise, overcome</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f9x4htr6f2hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1akq2nk</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>ILNP Vanity-found my fave purple</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yutlb7gx92hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1akoxxl</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>The Artist ✨️</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akoxxl</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1akit7x</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Swamp Gloss - But Elijah Wood, Part 2</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akit7x</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1akmt93</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>BKL and Mooncat are both releasing ghostly grey/pink shimmers this month in their new collections but it’s hard to imagine I’ll ever love one more than this Phoenix shade</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akmt93</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1akmk6y</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Valentine's Skittle 💕</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6eioz90zi1hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1akmie6</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Interesting combo, but idk if I like it on me</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akmie6</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1akmdj6</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Valentine’s Launches</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1akmdj6/valentines_launches/</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1akmbzl</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>I thought I got rid of my “purple problem” but turns out I just moved to another color.</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k343q23ch1hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1akm47d</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Ringing in the lunar new year with the closest thing I have to a red</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akm47d</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1akkv6r</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Thought I’d try this combo. It’s everything I hoped it would be</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akkv6r</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1akkutq</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Filing question</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1akkutq/filing_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1akk5am</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>What are these lines on the sides of my nails?</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lonq9cqv11hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1akjuo2</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Tried something new!</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akjuo2</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1akjraw</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Love any reason to show off my shades of red!</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r98xy9y2z0hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1akjocd</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Does this look intentional?</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akjocd</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1akjkw2</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Beautiful bottles?</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1akjkw2/beautiful_bottles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1akjbdi</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>My first set!</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akjbdi</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1akj8h9</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Doom for a Moody Vibe</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ou5lieefv0hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1akhoe6</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Red mani</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04d4fg06k0hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1akiq37</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>A Simple Girl with Simple Taste</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akiq37</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1akie05</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Drugstore Toppers</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k4i3o24dp0hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1akhkhi</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>such a gorgeous pink i could cry!</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akhkhi</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1akgxyj</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>80's Secretary Red With a Twist</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/V4wMwSO</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1akg0ma</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Graycloth</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akg0ma</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1akft02</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>First attempt at a love day mani</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5wz3tces60hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1akewa4</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>William Morris damask mixed green skittle 🥬💚🍏</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akewa4</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1ak12qh</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Getting into the jelly trend, first non-gel look in a while for me!</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ak12qh</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1akdygl</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Dashing Diva Nail Strips</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akdygl</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1akdavf</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>My color for the week: Throw It On (excuse the cuticles 😐)</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akdavf</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1akd5me</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Regular polish stays better than gels?</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1akd5me/regular_polish_stays_better_than_gels/</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1akcgp1</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Newbie here, tips??</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/objv7z3mhzgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1akcg3r</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Venetian Sky - Cirque Colors</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7334hyughzgc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1akccis</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Is it spring yet? (no)</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akccis</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1akbq03</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>what are your top 10 essential nail polishes or colors?</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1akbq03/what_are_your_top_10_essential_nail_polishes_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1akblt6</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Monarch Belladonna scratched the itch that Vanessa Molina Fishnet Stockings left for me</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akblt6</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1akbj34</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Nail art for the non-artist 🎨</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vp5p2x8iazgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1akb4jj</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Sassy Sauce knocks it out again</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ao2elula7zgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1akb3sw</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>overcast(ish) skittle</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akb3sw</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1akarwe</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Smashed thumbnail in door frame, now it has a crack in the center</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1akarwe/smashed_thumbnail_in_door_frame_now_it_has_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1akai5z</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Velvety glow ✨</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5xevh4182zgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1aka42w</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Anne Boleyn ♥️</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/83pmsh6zyygc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1aka1n0</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Valentine’s Day Skittle Mani</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aka1n0</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1ak99ql</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Had a polish party with a fellow lacquerista!</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ak99ql</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1ak8y5f</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>My first try at nail art, could be worse</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8xj89i6eoygc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1ak72hx</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Guess the polish</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3vjfiq8z3ygc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1ak5osh</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Learning to paint my nails after kicking the biting habit</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uzciibz6mxgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1ak55fm</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Once Upon a Time.....</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eyv3wx7zexgc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1ak51h9</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>This weeks mani</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gedvcpyhdxgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1akvebi</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Back again with the same colour combo!</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akvebi</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1akv727</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Valentines Nails</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qqnt3lbaj3hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1aktook</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Today's design for my client , spiral 💋💋💋</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h0hyidj453hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1akrcw7</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Vday nails done by me</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/newpvg4pk2hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1akpb7n</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Did some Valentine's nails!</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akpb7n</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1aknuug</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Valentine’s Day press ons 💕</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ttpqo6kjs1hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1aklvtd</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>I tried the coquette nail trend</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cuqt4ng3e1hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1akgtjq</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Valentine’s Day Nails ❤️</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akgtjq</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1akgilx</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>One set. Two colors. Red fish. Blue stripes.</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q2cdh93wb0hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1akdifl</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>What do you think about this design? 🦋</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e41qjpdrpzgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1akci5j</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Pink🩷</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akci5j</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1akbndo</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>My GF did my nails today</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3qf4a8bgbzgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1akangh</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Painted some smexy valentine's nails for myself 💗</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akangh</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Feb  8 08:07:55 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_02_11.xlsx
+++ b/data/2024_02_11.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C612"/>
+  <dimension ref="A1:C712"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10837,6 +10837,1706 @@
         </is>
       </c>
     </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1alg6g9</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>NYC: looking for a nail salon that keeps nails healthy</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1alg6g9/nyc_looking_for_a_nail_salon_that_keeps_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1alfb5b</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Valentine’s Day nails! 😁🩷🫶</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z1udvtihm8hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1ala1l1</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Lunar Year</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ala1l1</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1akzt6t</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>how important is dehydrator and primer?</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1akzt6t/how_important_is_dehydrator_and_primer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1akzcta</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Took inspiration from last night's post here..🤍❄️</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akzcta</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1akxbra</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Small gap between extension and nails - is this normal for nail extensions?</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akxbra</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1akw30m</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>press on nail advice</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2nxk4xxds3hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1akuwab</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Poly gel nails</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1akuwab/poly_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1al6hqh</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Not bad for a cute valentine look just think it could be better</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f0ow0gymt6hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1al6fh5</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Can I modify/add designs after I get my nails done?</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1al6fh5/can_i_modifyadd_designs_after_i_get_my_nails_done/</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1al4uzy</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>for under 2 bucks! i’m impressed 🤩</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yww3lrlyg6hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1al4m86</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>care bears set</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/stkrhg2ze6hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1al3o7n</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Valentines nails 👽</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i5y8s1k776hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1al2oyx</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>First rime trying press ons. Do they look alright? Any tips on preventing all those airbubbles?</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1al2oyx</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1al25ix</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>My current set!</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zzckn6gft5hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1al0s5q</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Where to start ? What technique to choose? Beginner recommendations :)</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gdjund3re5hc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1al04ar</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Can I soak off the gel polish from a gel tip, or the gel tip will also come off?</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1al04ar/can_i_soak_off_the_gel_polish_from_a_gel_tip_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1akz864</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>gaoy peel off base coat</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1akz864/gaoy_peel_off_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1alqnbt</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Subtle holo but so pretty!</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1alqnbt</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1alqn74</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Subtle holo but so pretty!</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1alqn74</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1alp3ij</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Anyone know the name of the topcoat I am looking for?</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1alp3ij/anyone_know_the_name_of_the_topcoat_i_am_looking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1aloqx4</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Velvetized Magnetic Skittle</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oozecc0cwahc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1alo58g</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Obsessed with this combo 💙</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v079wp20qahc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1alo41l</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>VDay nails</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/avixs4pnpahc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1alng9t</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Another reflective pink, because 'tis the season</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1alng9t</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1almwo9</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>moonfairy🤍</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m5vqyzftdahc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1alka8f</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>First skittle, V day experiment</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1alka8f</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1alazvv</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Happy with how my V-Day nails turned out 💌💌💌</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1alazvv</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1alm3xi</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Mooncat - Spaceoddity</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1alm3xi</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1alm2q7</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Finally broke out the Valentine’s stamping plates</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1alm2q7</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1alm11a</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Cirque new wave/ILNP birefringence?</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1alm11a/cirque_new_waveilnp_birefringence/</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1allylm</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>It’s over; all other magnetics are ruined for me</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pnnqa2105ahc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1allbqz</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Obsessed</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1allbqz</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1all20w</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Trying to choose a color for a costume--halp!?</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1all20w/trying_to_choose_a_color_for_a_costumehalp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1alkooa</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>ILNP Champagne Blush</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qoisn2int9hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1alk2kn</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>the aftermath of removing gel polish..</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1zgazpxho9hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1aljxga</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Nail polish dries/sticks to itself while I'm applying</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aljxga/nail_polish_driessticks_to_itself_while_im/</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1aljx0r</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Craving ILNP Poison but I'm on a no buy, so here's a deep red magnetic frankenpolish 😅</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yr2ycnn6n9hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1aljifz</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>What other "Glowy" polishes are out there that you recommend?</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8syokepoj9hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1aljean</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Starlight ✨</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wv4kfw7pi9hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1aljb8h</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>This polish reminds me of mermaid scales!</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ev24u86zh9hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1alivdz</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>I finally got an accurate color shift picture and I’m in awe</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1alivdz</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1alis4a</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Emily de Molly - Noxious</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1alis4a</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1alilh5</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Is there a polish put there that looks like the glitters in this popsocket? It doesn't have to have a pink like the background</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1alilh5</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1ali7yl</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Chill Purple Valentine Nails</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ali7yl</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1algrtg</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Lumen Glasswing Butterfly vs Lyn B Designs Gumdrop Mountains</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/of0m74tax8hc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1algemq</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>First attempt at nail art</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1algemq</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1alfste</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>What to paint first…</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1alfste</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1alexwk</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Spring flower (and a lil swamp) vibes</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1alexwk</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1alewq9</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>CND Leather Goods</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9yyi06njj8hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1aletrf</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Would any one have comparisons of Mooncat Mermaid Bait or Tectonic shift to Bees Knees There's Always Consequences or Twin Alders (pictured)? Newb to Indie Polishes, thnx!</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aletrf/would_any_one_have_comparisons_of_mooncat_mermaid/</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1aleslf</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Phoenix Bill (yes that’s actually the name)</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4qnrme1oi8hc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1alepiq</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>i felt like mooncatting this week</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1alepiq</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1alenjp</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Shimmer of many faces</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1alenjp</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1alecvi</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Recent mani roundup!</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1alecvi</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1alcmyv</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Forgive the 5 photos but this polish is so shifty and glowy it's impossible to capture in just one shot!</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1alcmyv</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1alck6v</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>A one coat nude for between more colorful nails?</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1alck6v/a_one_coat_nude_for_between_more_colorful_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1albns3</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Simple Valentines</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1albns3</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1albjy4</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>💗</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1albjy4</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1albi6a</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Now Hear Me Out... it's a neutral.</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1albi6a</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1albd1i</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>ILNP Carrie ❤️</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1albd1i</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1alatv6</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Trimming/filing for nails with strong c-curve and skin growing over nails?</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1alatv6</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1alaqc4</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Me buying this polish: “Wow, this topper is so unique!” Me adding it to my swatch ring: 🤦‍♀️</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5i23337jo7hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1alammg</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Lunar New Year Nails!! 🏮🍊</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1alammg</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1alaj6x</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Valentines Nails 💕💖🩷💓💓</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hcpcnp53n7hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1alaf18</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>For people who like their polish EXTRA smooth and shiny, what do you use?</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1alaf18/for_people_who_like_their_polish_extra_smooth_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1al9r5s</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Cirque Colors Perseus</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ou5n1x8ch7hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1alacwj</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Icy skittle (?) with BKL - The Sewers</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1alacwj</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1al9k1t</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>I wasn’t over these nails so I got them redone, this time in regular mani!</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5aumllqwf7hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1al9jy1</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Are there any tips and tricks to filing or cutting all your nails to a similar length?</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1al9jy1/are_there_any_tips_and_tricks_to_filing_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1al95v8</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>I found my blue glow holy grail</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/azgl7zd2d7hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1al8bco</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>chompers gonna chomp</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1al8bco</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1al87zm</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>This thermal is pretty cool♥️❤️🤍</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1al87zm</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1al7zry</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>New fav pale pink</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1al7zry</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1al7fu9</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Rogue Lacquer Bleeding Hearts (PPU Jan 24)</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1al7fu9</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1al73jp</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>anything similar to this that’s not a gel formula?</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7krl4h82y6hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1akxme9</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Trying to find a dupe</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akxme9</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1akxdlc</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>What shade is this please (Kylie Jenner’s nails)</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akxdlc</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1al6fw6</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Pinks &amp; Red for Feb: LNY Manicure #1!</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1al6fw6</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1al5wi8</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Taking good pictures of holo is so hard!</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a6uxdoi3p6hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1al528a</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>🖤❤️Leather &amp; Lace❤️🖤</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1al528a</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1al4div</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Moth to a flame</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/40kb9dm1d6hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1al4bao</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm still really new at doing my own nails - how do these look &amp; how can I improve?  </t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wd4qkogic6hc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1al45a2</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Low-budget magnet solution but I love the results!</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1al45a2</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1al3fmg</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Tried a brand that's totally new to me. 🤔</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/glv15bt956hc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1al37da</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>I’m getting better at this! One of my favorite sets I’ve done so far lol</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sexyu7i836hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1al369s</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Cherry Mocha Polish Recs?</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1al369s/cherry_mocha_polish_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1al1j17</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Had to go short, pretty sad about it.</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/MbSxrD3</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1akzgu1</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>My shower gel seems to discolor my nail polish, why ? And what can I do to remedy that ?</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/il0yrxhgy4hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1akyb0i</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Reminds me of Bath &amp; Body Works Cherry Blossom 🥰</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1akyb0i</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1almeim</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>A friend made these)</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p4uj59iy8ahc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1alm3gq</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Alex Gray inspired to go to see TOOL in concert, by @kalsrebelliousnails on IG</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/KbtiHPt</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1alljvw</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>set i made for valentines</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uhog9dza1ahc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1alli7x</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Pompompurin Cake Press-on Nails</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1alli7x</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1allfzv</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Valentine's Nails</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1allfzv</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1alhfdf</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Tried to make a video of my work for the first time. Let me know what you think! 🌉🌄😱🌊🌅</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lorzaht929hc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1ale8vp</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Valentine’s Day nails! ☺️🩷🫶</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cci8tz1me8hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1alc0b6</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Valentines nails !!</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0rd8dwn2y7hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1al7ner</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Goofy Goober Nails</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qt38109527hc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1al04aq</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>my valentine nails again - my reddit account got hacked..</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1al04aq</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Feb  9 08:07:32 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_02_11.xlsx
+++ b/data/2024_02_11.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C712"/>
+  <dimension ref="A1:C784"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12537,6 +12537,1230 @@
         </is>
       </c>
     </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1amag5h</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Tried acrylics for the first time!</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c94znyipbghc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1am4fp0</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>What step am I missing with my gel?</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1am4fp0/what_step_am_i_missing_with_my_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1alw12k</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Moons and stars 🌚</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ngiiuu88dhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1alqhtk</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Practising my hand painting</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d4ge8omrgbhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1amgdyw</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>LynBDesigns Sale?</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1amgdyw/lynbdesigns_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1amg9ka</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>More LynB Designs ~ One on each hand!</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amg9ka</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1amg96t</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Steel Your Heart (first attempt mixing my own polish)</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amg96t</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1amedws</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>INLP Eclipse is just a great color</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amedws</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1amcx63</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Felt compelled to paint my nails red to celebrate Lunar New Year / the Suberb Owl / Valentine’s Day ❣️</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amcx63</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1amcgf0</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Tết Nails!</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amcgf0</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1ambxx4</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Cadillacquer Winter Collection Pre Order?</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ambxx4/cadillacquer_winter_collection_pre_order/</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1amanva</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>I love it when my nails match things 🩵</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amanva</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1ama7cc</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>ISO help to not rip off my nails while sleeping 🥲</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ama7cc</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1am9zw5</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Kind of cool/weird ILNP combo</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1am9zw5</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1am9jjw</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Calling this one “Blood and Chocolate” ❤️🥀🍫🤎</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1am9jjw</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1am8810</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>KBS - Lights Out</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7t0uzqyytfhc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1am87c3</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>we kinda match</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3pnhrq7vtfhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1am5q5a</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Thermal Valentine’s Nails</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wqnih4l6bfhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1am7rpy</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Tenta cool vs Don't Provoke Me</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1am7rpy/tenta_cool_vs_dont_provoke_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1am7p8b</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Nothing says valentine's month like royal blue China 💙🍽️</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1am7p8b</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1am7ir1</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>A student told me my nails look like “an alien threw up on them” 👽</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1am7ir1</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1am7h56</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>New to nail obsession, some questions</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1am7h56/new_to_nail_obsession_some_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1am76ku</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Kind of vday inspired</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j2ss6rk5mfhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1am6ojc</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>First try with super cheap press-ons</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oub2wghcifhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1am6ntn</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Rosewater Jelly with a lil something Sassy</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1am6ntn</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1am6i7o</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Tried nail art for the first time… it was much cuter in my head</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1am6i7o</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1am68lu</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Spellbound Nails</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1am68lu/spellbound_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1am658t</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Valentine's Day skittle 🩷💜</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w7dy64xbefhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1am5oib</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Totally fan- girling....</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/51cu2lmtafhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1am54g7</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Did anyone get the Zoya Love polish?</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1am54g7/did_anyone_get_the_zoya_love_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1am4t3d</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Any more opaque/matte "Boring" flakie toppers out there?</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1am4t3d/any_more_opaquematte_boring_flakie_toppers_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1am4atu</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>🩷💙Neon Hearts💜💛</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1am4atu</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1am46vv</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>OPI - Kyoto Pearl</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fbg66sfqzehc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1am3t4a</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Any reviews on Essie special effects line?</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1am3t4a/any_reviews_on_essie_special_effects_line/</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1am3nuf</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Subtle Valentines nails ❤️</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1am3nuf</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1am3b2f</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Arctic Fox "Cosmic Sunshine" + Holo Taco "Lunar Unicorn Skin"</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h9w8z011tehc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1am2kzj</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Multichrome Gradient</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/seincgjnnehc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1am2kmj</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Lovestruck Collection Valentine’s Day mix n match mani 🥰 (PR - gifted)</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1am2kmj</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1am2gjn</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>silver nail polish has my heart</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ksafodqmehc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1am2buq</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>ILNP “Love Language”</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2n3zfrerlehc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1am27t7</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Palate cleanser :P</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xmvosw3ykehc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1am25m0</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Any Mooncat Snake Charmer dupes out there?</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1am25m0/any_mooncat_snake_charmer_dupes_out_there/</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1am21qu</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>First attempt at nail "art"</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/orivcn8pjehc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1am1u3r</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>It’s beautiful but AT WHAT COST (also I would love recs for more vampy shades with red shimmer)</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1am1u3r</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1am0k4y</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Wildflower Lacquer Dark Beauty (PPU Jan 2024)</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1am0k4y</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1alzott</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Mooncat Shattered Glass</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1alzott</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1alyfyz</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Barb from Sassy Sauce</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l4csvcsfsdhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1alxgva</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>blue/brown duochrome polish?</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ge1yhchmkdhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1alxeiv</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Spirited Away Studio Ghibli Nails 👻🐉🐖🐀⚫</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1alxeiv</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1alxc6h</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Polished for Days I Had Wings Once</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bfd4vb0kjdhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1alx8z9</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>first time attempting french nails</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1alx8z9</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1alx6w8</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>The color is subtle, but that holo...</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zxh1mrnbidhc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1alwvku</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Sheer pink mani</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/18doe83qfdhc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1alp72m</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Does anyone know how to clean up nail polish thinner?</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1alp72m/does_anyone_know_how_to_clean_up_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1alt2us</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Can you tell pink is my favorite color? 🩷🌸🌷🎀 Polishes listed below</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1alt2us</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1alv0kb</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Wall Reorganization Day!</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nbbo5fb3zchc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1amiahv</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Valentines nails 🩷</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amiahv</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1amg6jb</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Silver heart nails 🩷🤍</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amg6jb</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1amejtq</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Hand painted</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3znzgwcebhhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1amcbu4</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Valentine’s Day nails 💅🏼</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amcbu4</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1ambx1u</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Fnaf nail art</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ambx1u</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1amahji</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>i suck at making a decision🥲😅</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amahji</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1am9fcs</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Scooby Doo</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/48798k5e3ghc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1am8mzf</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>did my valentine‘s day nails today🤍</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/72di1oc7xfhc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1am54z0</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>another vday set for your feed 🙈</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1am54z0</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1am4jmg</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>My hand painted press-on nails.</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1am4jmg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1am141k</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Cold but comfy</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1am141k</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1am109z</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>New set I did. Wearing a gold and green dress to a wedding this weekend and didn’t want traditional valentines colors to clash</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1am109z</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1am0bnh</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Self taught</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1am0bnh</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1alyczq</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Why is my nail foil peeling and scratching off? Issue with the glue?</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1alyczq/why_is_my_nail_foil_peeling_and_scratching_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1alwyqj</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Animal print for my client from earlier today</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/deajo7xggdhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1alwn9k</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Moons and stars ✨</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p0x43yrrddhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Feb 10 08:06:43 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_02_11.xlsx
+++ b/data/2024_02_11.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C784"/>
+  <dimension ref="A1:C915"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13761,6 +13761,2233 @@
         </is>
       </c>
     </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1anaju0</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Valentines but black</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anaju0</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1anab8r</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Valentine's day theme. How many hearts do you see 😉</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wngspc7tgphc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1ana91z</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>First try. Pop art</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/c35zsy33gphc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1ana4cj</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>my valentine’s set! 💌</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/omitp43lephc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1an9dot</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Inspired by one of the top posts from this sub 💕</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hnkbmnwe6phc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1an9rez</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Valentine’s day nails</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1an9rez</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1an9ok6</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>a gel x set i did today!</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mt0thdum9phc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1an9au3</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Classic 🤍</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u3qe6obi5phc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1an9a96</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Split nails 😩</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1an9a96</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1an96b1</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Cherry 🍒 nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wbobp6b54phc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1an8y80</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Anti slip steel plate nail art</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1an8y80</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1an5vwi</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Soft/Brittle Nails After Acrylic Removal</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1an5vwi/softbrittle_nails_after_acrylic_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1an8qh0</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>whats an acrylic overlay?</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1an8qh0/whats_an_acrylic_overlay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1an15kj</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>What happens if I put new nail glue + acrylics on top of old nail glue that won't come off?</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1an15kj/what_happens_if_i_put_new_nail_glue_acrylics_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1an4jr2</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Salon accidentally cut side of nail too short, how can I prevent ingrown nail?</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qti4f4llvnhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1an7ybd</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Valentine’s mani! My third time doing my own dip nails 🥳</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1an7ybd</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1an7wkv</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Valentines Nails ♥️</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1an7wkv</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1an7uff</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Spider lily and dragon new year 🩶</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m1tjf03mqohc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1an7p8h</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Valentines nails!</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04spupa5pohc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1an75eb</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Cute?</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6cy7uyyrjohc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1an7528</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>I’m not used to long nails, so I figured I’d start with press-ons ✨</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1an7528</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1an74fo</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Simplified Black Coquette Style 🖤</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1an74fo</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1an6p9x</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>My nail tech did me good</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7ka09954fohc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1an5qq1</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Valentine's day nails</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1an5qq1</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1an5kkt</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>airbushXXXchrome</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bcyla3bl4ohc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1an49dj</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Inspired by a post I saw here!</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0t7ff293tnhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1an5i8m</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Valentine's Day</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1an5i8m</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1an5aqd</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Idk why I was expecting her to draw the 🦋</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vhil31t42ohc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1an53bq</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Matte Gray Sparkle ✨</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1an53bq</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1an4h8z</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>First time getting acrylics (no idea how they come off though)</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/824qk4tzunhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1an49lf</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Valentines day nails 💕</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1an49lf</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1an401a</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Question about structured manicures</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1an401a</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1an3j2v</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Catching prey, not feelings, with my Valentine's Spider nails.</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oxwg1ngsmnhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1an38ia</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Red French for Valentines 💘</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y6o2j0dcknhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1an36s9</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Am I on the right track?</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1an36s9</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1an36if</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Gel French tip</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5gczh3mvjnhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1an2k53</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Shorties 😍🌸🎀</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1an2k53</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1an1oql</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Valentines nails :)</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/axb735en7nhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1an1fog</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>For at-home gel manicures: can I put nail stickers with top coat under the UV light??</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1an1fog/for_athome_gel_manicures_can_i_put_nail_stickers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1an15jo</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Horrible 😭</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1an15jo</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1an0gyi</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Does anyone have any ideas for grunge nails?</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1an0gyi/does_anyone_have_any_ideas_for_grunge_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1amy4xe</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>My Cheshire cat set ♡</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amy4xe</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1amro71</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Still so into abstract!</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amro71</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1amnx4t</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Inlove with my Hello Kitty set ♡</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d1lvjvwb8khc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1amnr9q</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>My Valentine’s Day nails 💋</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amnr9q</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1amlp8i</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Kiki’s Delivery Service</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/agvodgyvkjhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1amaqqb</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Half moons, glitter and hearts 🌙✨️❤️ inspired by @heygreatnails on insta!</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amaqqb</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1am8rzy</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Valentine’s Day Nails</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1am8rzy</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1anafg0</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Drugstore shade similar to this?</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lsh7txe6iphc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1an9ud8</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Heartbreak doesn’t even begin to describe it…</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1an9ud8</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1an9gzy</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Base coat convert</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1an9gzy</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1an8wq1</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Vday nails (:</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/26jb4tt91phc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1an8wg5</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Loving this hot pink 🩷</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lakeiqy61phc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1an8sss</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Perfect black</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1an8sss</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1amx2wf</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>I tried to paint Celeste from Animal Crossing</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/psiazi5y7mhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1an876z</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Can I see your wedding nails? And did you do them yourself?</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1an876z/can_i_see_your_wedding_nails_and_did_you_do_them/</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1an82uv</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>What could be causing my nails to get dry and cracked like this?</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1an82uv</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1an7iz7</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>What causes a single nail to delaminate non stop?</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/399fb6wfnohc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1an79sb</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>I love pink and red together 🥰</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jd607r2ykohc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1an77m4</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>My non-popular take on vday and lunar new year nails</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/33l9741dkohc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1an6mfs</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Luxapolish Convert</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1an6mfs</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1an5v40</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Soft/Brittle Nails After Acrylic Removal</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1an5v40/softbrittle_nails_after_acrylic_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1an4yp9</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Looking for a dupe!</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1an4yp9</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1an4sdk</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>New nail mail arrived!</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0l2pp4soxnhc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1an4h49</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Sour</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1an4h49</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1an3dmz</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Overcast lighting really makes nails pop</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w18hvt6ilnhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1an2d1h</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>I love black with flakies but I jazzed it up a little bit with a turquoise peek.</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1an2d1h</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1an27j6</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Sheer skittle</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1an27j6</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1an21zx</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>did these for valentine ❣️</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1an21zx</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1an13xp</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Neon pink and blue bc I need summer</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lztilih53nhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1amzz65</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Looking for a color like this! I have pink goldfish from olive and June I just wish the shift was pink.</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/omf6erlbumhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1amzeon</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>damaged nail beds</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1amzeon/damaged_nail_beds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1amz4ik</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Blazing Star like a Blue Morpho 🦋</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amz4ik</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1amz3a0</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Apparently I need to bring my swatch sticks everywhere I go</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dw9c5fqfnmhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1amz2jk</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Kiss Me, I’m Pretty (and I just might)</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d5hcsqv9nmhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1amy3pv</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Coral Chaser</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u1yjhspvfmhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1amxxv9</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Bee’s Knees Lacquer I’m Fast, Very Fast QDTC - Opinions?</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1amxxv9/bees_knees_lacquer_im_fast_very_fast_qdtc_opinions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1amxmeq</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Rhinestone party Valentine’s Day nails by me 🩷❤️✨</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amxmeq</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1amxk0h</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Attempted Lunar New Year Nails</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amxk0h</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1amxj5y</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>In love with this match!</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amxj5y</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1amx4v4</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Holographic hearts 💖</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amx4v4</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1amwnbt</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>One coat of Mooncat moonjelly for that spa day/refresh vibe 😌🧘‍♂️ tried to capture all the shimmer!</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amwnbt</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1amwivm</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Adding in my Lunar New Year nails! 🧧🐉 🏮</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amwivm</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1amw6uz</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Mooncat - Velociraptor</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amw6uz</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1amw2lv</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>My new love: LynB White Chocolate</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amw2lv</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1amvnn6</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>V-Day Nails 💖</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amvnn6</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1amvmlt</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Birthday mani!</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qul8i08ywlhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1amvflu</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Valentine stubs</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k87y2kwgvlhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1amvblb</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Nail art — Take 2</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amvblb</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1amv4z6</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Lunar New Year Nails 🧧 Year of the Dragon!</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amv4z6</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1amuxkz</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Moody Valentine 🥀</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amuxkz</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1amupj4</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Are press ons really that bad for your nails?</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1amupj4/are_press_ons_really_that_bad_for_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1amumys</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>First Try at Velvet</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amumys</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1amu8lp</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>My nails are in rough shape from decades of picking, but 2 weeks ago I finally began my nail care journey and have just received a new delivery of polishes!</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zvft299hmlhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1amtwcm</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>The 'Change of Plan' mani</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/PuS8f8i</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1amtmz2</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>OPI Repair Mode</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1amtmz2/opi_repair_mode/</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1amtk26</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Sometimes you just can’t beat a classic red.</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8absgewchlhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1amsn24</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Is it possible for my nails to be both strong and flexible? Having builder gel troubles</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1amsn24/is_it_possible_for_my_nails_to_be_both_strong_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1amsk8j</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>This shade is just gorgeous!</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uh9po4y3alhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1ams7h8</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Here we go....Firefly forest....</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cysj6xfi7lhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1amd0b1</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Inadvertently did Lunar New Years nails!</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amd0b1</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1amrvwc</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Excuse the messiness, but this combo is so glowy😍</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b2c4om345lhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1amrvjk</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>I can't stop staring at my nails!</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q6cpfjj15lhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1amrbbi</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Ladybug + Cat Noir Nails</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dkdgw3uu0lhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1amqz4i</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Back with more music inspired nails!</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amqz4i</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1amqwtd</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer - SHOW US YOUR MANIS!</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1amqwtd/lurid_lacquer_show_us_your_manis/</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1amqex5</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Fresh chop ✂️</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dyutc7eqtkhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1ampzwn</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Why do my gels always lift in the corners after a couple days?</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ampzwn</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1ampdha</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>They're giving: Valentine princess 👸 What do you think?</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ampdha</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1amp70j</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Wild Berry West! 🍓🫐🤠</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amp70j</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1ammqd8</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Pray for me: My collection was stuck in a -26°C/-14.8F warehouse for two weeks and all bottles froze</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ftttnxsgwjhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1amlbi9</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>New mani for Dutch carnaval</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amlbi9</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1amj11b</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Looking for magnetic recs available in aus</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1amj11b/looking_for_magnetic_recs_available_in_aus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1an8wvw</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>You will never catch me slippin</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1an8wvw</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1an83ml</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Today flowers for my client 🥰🎀🌸🌸🌸</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r946ld45tohc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1an6mer</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Lunar New Year nails made by me🧧🏮</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1an6mer</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1an6khv</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Valentine's Day Nails/Goth Inspired</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/46su6f30eohc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1an4t8v</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Zebra design nails 💗</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qcadi9otxnhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1an4lzp</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>My Valentine’s Day nails🤍🩷</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7r2ouy55wnhc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1an3gt3</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>My set this week</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1an3gt3</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1an0hsk</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Red and gold set</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1an0hsk</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1amyap5</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Valentine's set with gradient chrome hearts</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amyap5</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1amxk9y</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Rhinestone party Valentine’s Day nails by me ❤️🩷✨</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amxk9y</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1amw1n3</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Hand painted clouds :)</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gf1r0zl50mhc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1amshyk</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>I'm so proud and in love with these cat themed nails 😍</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amshyk</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1ams036</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>14 February nails 💋</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ams036</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1amrubm</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Green &amp; Gold under different lighting</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1amrubm</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1amolse</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t xml:space="preserve">More cat eye shenanigans! </t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0764yx7mekhc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1ammu10</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Valentines nails</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/moxy6e6hxjhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1amm5l3</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Kiki’s Delivery Service</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6oxu1i38qjhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1aml7va</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Valentines but make it black 🖤</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aml7va</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Feb 11 08:07:07 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_02_11.xlsx
+++ b/data/2024_02_11.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C915"/>
+  <dimension ref="A1:C1077"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15988,6 +15988,2760 @@
         </is>
       </c>
     </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1ao26v0</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Ode to the 🌊</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ao26v0</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1ao23mb</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Lunar New Year Nails</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/itzz32r8owhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1ao19i2</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>What shade from Gelish is this?</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ao19i2</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1ao16dd</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Love my Valentine’s set.</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ao16dd</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1ao12xg</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Valentine sets I did</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ao12xg</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1ao0vfp</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>my valentine nails 🥹</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p0ack3trawhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1ao0o5s</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>are these almond?</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vwwn05cl8whc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1anync8</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>How do I take off nail glue from the back of my fake nail!!</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1anync8/how_do_i_take_off_nail_glue_from_the_back_of_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1anx6x3</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Dark pink for Valentine’s, can u tell?</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a7kj37r0avhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1anvk0h</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Titanic/Heart of the Ocean inspired 💙 Structured manicure overlay done with hard gel on my client’s natural nails ✨</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anvk0h</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1anuscl</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Suggestions for splitting nail?</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1anuscl/suggestions_for_splitting_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1ao07vq</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Im new to using gel, and tips, how is my first time doing them? (ps, im still shaping these😭)</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/731m489q3whc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1anrzgx</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>What nail design should I go with for a winter formal?</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1anrzgx/what_nail_design_should_i_go_with_for_a_winter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1anzp95</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>manucurist nail glow</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s97t9padyvhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1anz5zt</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Tried a DIY leopard and can’t believe how it turned out</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o4c9psowsvhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1anz2f9</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Does anyone have a shade match to this color? Preferably gel?</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/weccjy6wrvhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1anyn5g</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Peep the new Valentine’s Day nails 🩷</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tdcb3xjqnvhc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1any3m0</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail gradient </t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/09chu0biivhc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1any0y7</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Can I use a regular UV lamp for gel polish?</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1any0y7/can_i_use_a_regular_uv_lamp_for_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1anxxpa</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>🤍🖤</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anxxpa</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1anxqid</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>finally tried…</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qbmu6vr4fvhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1anxjpp</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>In Lovee!</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anxjpp</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1anxfpk</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Lilac with blue chrome</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uh7o73cbcvhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1anwys3</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>First time trying out slider stickers, what do you think? 👀</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anwys3</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1anwrru</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>VALENTINE'S SET</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k7fsfr406vhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1anwm4c</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Back on my DIY game just in time for V-day!</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anwm4c</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1anwdwz</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy Lunar New Year 🐲 </t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e24qyl6e2vhc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1anmwe7</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>What should I do for my wedding?</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1anmwe7/what_should_i_do_for_my_wedding/</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1anw7q8</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>my most favorite set yet!</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ygke8ow0vhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1anvyal</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Stole the design ! Beautiful!</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uxtbzt3iyuhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1anvjyl</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>February set</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dbz9xjc1vuhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1anvgcr</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Valentines Day nails</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anvgcr</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1anvf7t</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>🖤</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anvf7t</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1anvain</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Does this color compliment my skin tone okay?</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anvain</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1anv92b</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>V-Day Dino Press-ons!</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cyg0ap2hsuhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1anv88y</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Valentine’s Day nails p.2 💕</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anv88y</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1anupnl</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>V-Day Nails</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sdnqiobvnuhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1anudv6</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Valentine Aura nails 💗💗</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hmj0fu94luhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1anu9t1</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Pink tips 💖</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0tredex6kuhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1anu94d</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Orlando Magic nails</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anu94d</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1anu2za</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>after a professional japanese gel manicure - could i add my own nail art? how?</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/obsko7zliuhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1antj0g</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>First time doing nails!</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1antj0g</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1antdnc</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Valentine’s Nails while everyone’s sharing theirs! 💌</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8fs1yjkscuhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1antc8i</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Paint Splatter/ Marble</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h7ne2z9fcuhc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1ant6nk</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Valentines set done by my nail tech 💖 acrylic overlay</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8avmo7p7buhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1ansx25</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Mickey Mouse</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hytkqmc69uhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1ansttm</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Nail tech did a nice job on my dip Valentine’s Day nails :)</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dpr07dve8uhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1ansp8l</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Valentine’s nails 🖤</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/va8dm6ce7uhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1ansbay</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>advice on gel x sizes and shapes</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ansbay/advice_on_gel_x_sizes_and_shapes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1anry92</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>which nail shape suits my hands the best</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anry92</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1anrvb9</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>I love sheer nudes</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ehe1ckq0uhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1anrnuv</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Favorite top coat?</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1anrnuv/favorite_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1anrnjl</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>gel x nail set i did!</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2pbgf6ozythc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1anrj5g</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Pink for Valentine's Day, nothing fancy but I like the bold colour</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aml3b5s5xthc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1anr5si</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>V-day set 💌</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anr5si</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1anr1oc</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>New to cuticle care</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gzbu4tn7uthc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1anqyyu</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>New set 💕💕</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3i790ywltthc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1anqw93</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>help 🙏</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1anqw93/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1anqnej</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>My Valentine's Day Set! (tech is @ skittcraft_beauty)</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anqnej</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1anqibn</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Actually so proud of this set I did on myself considering I haven't done nails since October! Still need electric file for small imperfections</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anqibn</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1anop6h</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>What tool is this?</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/70rfg32kbthc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1anp7e5</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>MIFFY NAILS for Japan Trip</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anp7e5</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1anp2qa</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Today's nails!</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u6d78jofethc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1anoq2o</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Got my nails done for the first time 🥰 such a cute design for valentine's day 💘.</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qo5wyttqbthc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1anoj19</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>valentines nails on myself!</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anoj19</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1annmkp</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>something about animal print</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rlb59b753thc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1ann40v</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>When you do a cute polish combo but can't remember what you used</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0buh05o1zshc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1anmv3t</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Velvet ribbon nails for Valentine’s using mooncat velvet rose</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anmv3t</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1anmizy</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Violet is my pasión</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lcgjc0tgushc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1anm39w</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>New set. Thought I’d try something different! 💕</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f7y3yhz0rshc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1anm1pk</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>I like it when my hands and feet combine</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r05enpgpqshc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1anm16m</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>spent so long growing out my nails 😭😭😭😭😭</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q6t1pxblqshc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1anlstu</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>🩷</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/12w9np3roshc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1anlnok</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>first time getting my nails done 🥰</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/313l3twlnshc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1anla6f</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Went to my moms Russian manicurist and she did not disappoint</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anla6f</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1anl1di</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Dark red/cherry cola nail polish</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1anl1di/dark_redcherry_cola_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1ankuer</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Nails for Valentine’s Day</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ankuer</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1ankr38</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Here is my baby Groot ♡ (Acrilic Painting)</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7xrk7qiqgshc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1ankn95</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>🤍</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7aoyaz4ufshc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1ankejb</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Semi-clean girlie</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0glfibbvdshc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1ank0d8</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Kabuki Inspired Nails</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ank0d8</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1anjjzp</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>need advice going from gel to non-gel</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anjjzp</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1aniufa</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>VDay Nails ✨ Credit @angiesclawss on IG</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aniufa</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1ank1o1</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Rainbow aura manicure 💅✨</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ank1o1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1ank01u</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>I LOVE my nail girl 💜✨</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ank01u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1anjlwn</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Obsessed is an understatement!</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jrhpwowd7shc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1anjl3j</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Valentine’s Nails</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anjl3j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1anj7ks</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>"Look Shadow, it's you!"</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anj7ks</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1anj0wj</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>another mani with boo</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h9vn42nr2shc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1anibb7</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>What do I want?</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1anibb7/what_do_i_want/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1ani7vz</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Stamping Question - Large Etched Areas</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fvcwccr1wrhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1anhru9</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Why does my nail grow like this? Is there anyway to prevent it? This is the only one like that</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ia71jv19srhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1anb3tw</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Hate my nails - can anyone give me advice with how to fix them up? My nail beds are rounds and my cuticles always peel</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anb3tw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1anb2hx</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Valentine's pop 🎨 ➡️</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anb2hx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1aniiz4</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>valentine’s day nails ◡̈</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8u8awgcoyrhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1an9w0v</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Why does this tearing/splitting happen at the sides with hard gel?</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1an9w0v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1angges</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>My first try on pop art nails</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1angges</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1ang19f</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Why did this happen? (Lazy Girl Polygel)</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ywm2dqjcrhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1ane4vw</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Made French manicure for the first time</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2i7ptdq3sqhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1ands8e</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>V-Day Nails 💕🎀</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ands8e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1ao22bj</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Tell me your fav magnetics!</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ao22bj/tell_me_your_fav_magnetics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1anzk9q</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>V-Day Mani 💕</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mngbpm4ywvhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1anrmnq</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Gel top coat has very strong odor? Is this normal?</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1anrmnq/gel_top_coat_has_very_strong_odor_is_this_normal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1ant1pl</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Here's the millionth post about Dragon Scales!</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ant1pl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1anzbtp</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Olive &amp; June Alternatives</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1anzbtp/olive_june_alternatives/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1anyuhr</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Hard Candy-Death Valley</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anyuhr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1anyoaq</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Resin mix-ins from the Dollar Tree craft section have potential…</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anyoaq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1anyc4f</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Nailtiques Day 1</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anyc4f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1anxqv6</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Holo Taco combo</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mmnbk588fvhc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1anxmur</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Non-dominant hand pictured!</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c3d8bso5evhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1anxka8</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Help! Which one should I do this week!</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anxka8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1anx24k</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Mani #5: The Piece de Resistance...</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anx24k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1anwz8u</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Quinlan 🥰💕</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anwz8u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1anwz6s</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>How about nails but they’re ✨transparent✨</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anwz6s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1anwppn</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>My first time ever attempting this. I’m happy with how it came out!</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anwppn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1anoxg6</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Polygel Nails and Eye Corner Scratching</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1anoxg6/polygel_nails_and_eye_corner_scratching/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1anwahn</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Guuuuys, pixie party is amazing ✨</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anwahn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1anw1zn</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>So Proud</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anw1zn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1anw1jq</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>OBSESSED with reflective glitter top coats 😍</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hjhzhsubzuhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1anvx7g</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Valentine’s Day nails🥀</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hbwncb09yuhc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1anvoi7</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Tried using a striping brush for the first time to make thin lines</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cro7mlk4wuhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1antz0p</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>ILNP Birefringence</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rxottwsdhuhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1antflt</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>LynB - Puppy Kisses 🐶</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1antflt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1ansfjx</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>The many faces of Phoenix Boolba</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ansfjx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1ans8of</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Can't stop, won't stop, staring at my nails.</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ans8of</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1ans82h</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>yet another vday nail art</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ans82h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1ans7c6</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Happy Lunar New Year! 🧧</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ub9im23g3uhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1anrl8j</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>I’ve been trying to take better care of my nails. Today’s mani!</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q2icokfiythc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1anre21</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Rewearing Ether Dragon on longer nails 🐉</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anre21</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1anr72c</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>valentine’s holo!</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anr72c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1anr4j2</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Valentine's Day hearts 💞</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/22mv6e9vuthc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1anpxcr</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Anyone wanna talk about new Mooncat collection??</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1anpxcr/anyone_wanna_talk_about_new_mooncat_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1anpqc7</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Question about hard builder gels from a gel polish DIYer</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1anpqc7/question_about_hard_builder_gels_from_a_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1anphuk</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>even more Lunar New Year nails 🐉🎆</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anphuk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1anp44z</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Got bored 2 days into a mani, added a topper.</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anp44z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1anoztk</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Neutral with a twist</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anoztk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1anodef</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Rounded replacement brushes for OPI gel polish?</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1anodef/rounded_replacement_brushes_for_opi_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1anob9y</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Is anyone else over quick dry top coats?</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1anob9y/is_anyone_else_over_quick_dry_top_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1annlgk</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Confused by this baggie of pigment</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1annlgk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1anmzig</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Velvet/cat eye hybrid for valentine’s</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anmzig</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1anl6n4</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Ready for Valentines 💌</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anl6n4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1anknmq</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Picture Polish Mulberry is my new favorite</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/djr8ge4tfshc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1anjuve</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Ready for Valentine's Day with Mooncat Your Heart's a Black Hole</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s71vchve9shc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1anjpfa</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Polish Collection</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anjpfa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1anj91o</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Valentine's choice</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anj91o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1anifcm</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>I think I found my favorite pink</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04w0dr0sxrhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1anfbp9</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Went for my favourite red</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0n745noc5rhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1ane19n</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>How do yall avoid bubbles in your topcoat</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ane19n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1and9bz</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Charm gel recommendations + tips</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1and9bz/charm_gel_recommendations_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1ancbmy</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>happy lunar new year everyone :)</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5h6ue05i5qhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1ao25hj</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Nail art for my 21st birthday 😍</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/okqocfktowhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1ao22yv</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Lunar New Year Nails</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zhvrql71owhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1ao039e</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>What do you think about my hand painted?</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4c9iqgoc2whc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1anze12</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Phantom of the Opera nails</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anze12</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1anwegn</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy Lunar New Year 🐲 </t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n1bgv6fj2vhc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1anwcto</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Valentine’s nails!!</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7zmuw5b62vhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1anw6t4</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>First Valentine’s Day nails ever</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/osfbp2on0vhc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1anv9uy</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Painted flowers on myself 🌸🌷</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anv9uy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1anv8yp</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>I’m new at doing my own nails, especially nail art. This is the first time it actually came out decently. What do you think?</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1anv8yp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1annrli</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Valentine’s day nails ♥️🎀🌟</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x9nlg9r84thc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1anmj1e</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Valentines nails</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4pknap7hushc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1ankdtj</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Kabuki Inspired Nails</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ankdtj</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>